<commit_message>
Added tables to the 'More information' window
</commit_message>
<xml_diff>
--- a/climate_impact_taxonomy.xlsx
+++ b/climate_impact_taxonomy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub.sharepoint.com/sites/eceprog/Shared Documents/Projects/CWF/SCIL_2024/Taxonomy/Taxonomy update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\streamlit_taxonomy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1088" documentId="8_{5D6BC7B4-9D3F-4CE7-B6E2-3FB5F782E196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8640447-E2BE-443D-A75B-FEE730F55C5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CC6328-EE25-453F-ADA3-B49FC850AE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28515" yWindow="795" windowWidth="24735" windowHeight="14475" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -9294,7 +9294,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9575,9 +9575,6 @@
     <xf numFmtId="0" fontId="21" fillId="26" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="26" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -9598,6 +9595,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="26" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9626,21 +9626,6 @@
     <xf numFmtId="0" fontId="23" fillId="35" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9665,8 +9650,35 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -10163,8 +10175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D5865F-5FC4-4B94-9D02-258B63D94AF6}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -10203,37 +10215,37 @@
         <v>2803</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="96" customFormat="1" ht="15.75">
-      <c r="A6" s="97" t="s">
+    <row r="6" spans="1:7" s="95" customFormat="1" ht="15.75">
+      <c r="A6" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-    </row>
-    <row r="7" spans="1:7" s="96" customFormat="1" ht="15.75">
-      <c r="A7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="97"/>
-    </row>
-    <row r="8" spans="1:7" s="96" customFormat="1" ht="15.75">
-      <c r="A8" s="99" t="s">
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+    </row>
+    <row r="7" spans="1:7" s="95" customFormat="1" ht="15.75">
+      <c r="A7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+    </row>
+    <row r="8" spans="1:7" s="95" customFormat="1" ht="15.75">
+      <c r="A8" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="99" t="s">
+      <c r="C8" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="99" t="s">
+      <c r="D8" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="99"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="97"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="96"/>
     </row>
     <row r="9" spans="1:7" s="85" customFormat="1" ht="25.5">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="94" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="93" t="s">
@@ -10250,7 +10262,7 @@
       <c r="G9" s="86"/>
     </row>
     <row r="10" spans="1:7" s="85" customFormat="1" ht="25.5">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="124" t="s">
         <v>2801</v>
       </c>
       <c r="B10" s="69" t="s">
@@ -10267,7 +10279,7 @@
       <c r="G10" s="86"/>
     </row>
     <row r="11" spans="1:7" s="85" customFormat="1" ht="25.5">
-      <c r="A11" s="68"/>
+      <c r="A11" s="125"/>
       <c r="B11" s="93" t="s">
         <v>2755</v>
       </c>
@@ -10282,7 +10294,7 @@
       <c r="G11" s="86"/>
     </row>
     <row r="12" spans="1:7" s="85" customFormat="1" ht="25.5">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="127" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="69" t="s">
@@ -10299,7 +10311,7 @@
       <c r="G12" s="86"/>
     </row>
     <row r="13" spans="1:7" s="85" customFormat="1" ht="25.5">
-      <c r="A13" s="70"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="70" t="s">
         <v>17</v>
       </c>
@@ -10312,7 +10324,7 @@
       <c r="G13" s="86"/>
     </row>
     <row r="14" spans="1:7" s="85" customFormat="1" ht="38.25">
-      <c r="A14" s="70"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="69" t="s">
         <v>19</v>
       </c>
@@ -10327,7 +10339,7 @@
       <c r="G14" s="86"/>
     </row>
     <row r="15" spans="1:7" s="85" customFormat="1" ht="25.5">
-      <c r="A15" s="70"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="70" t="s">
         <v>22</v>
       </c>
@@ -10340,7 +10352,7 @@
       <c r="G15" s="86"/>
     </row>
     <row r="16" spans="1:7" s="85" customFormat="1" ht="25.5">
-      <c r="A16" s="68"/>
+      <c r="A16" s="128"/>
       <c r="B16" s="93" t="s">
         <v>24</v>
       </c>
@@ -10443,7 +10455,7 @@
       <c r="D23" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="100" t="s">
+      <c r="E23" s="99" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="73" t="s">
@@ -10667,7 +10679,7 @@
       <c r="F39" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A2:XFD2"/>
@@ -10676,6 +10688,8 @@
     <mergeCell ref="A5:XFD5"/>
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10687,7 +10701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1248"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -10731,45 +10745,45 @@
       <c r="A1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="111" t="s">
         <v>2801</v>
       </c>
-      <c r="C1" s="116"/>
-      <c r="D1" s="118" t="s">
+      <c r="C1" s="111"/>
+      <c r="D1" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="117" t="s">
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="118" t="s">
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="P1" s="112"/>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="112"/>
+      <c r="S1" s="113" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="118"/>
-      <c r="U1" s="118"/>
-      <c r="V1" s="118"/>
-      <c r="W1" s="117" t="s">
+      <c r="T1" s="113"/>
+      <c r="U1" s="113"/>
+      <c r="V1" s="113"/>
+      <c r="W1" s="112" t="s">
         <v>70</v>
       </c>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="111" t="s">
+      <c r="X1" s="112"/>
+      <c r="Y1" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
+      <c r="Z1" s="119"/>
+      <c r="AA1" s="119"/>
+      <c r="AB1" s="119"/>
     </row>
     <row r="2" spans="1:28" s="2" customFormat="1" ht="18.75" customHeight="1">
       <c r="A2" s="26"/>
@@ -10780,76 +10794,76 @@
       <c r="F2" s="52"/>
       <c r="G2" s="52"/>
       <c r="H2" s="26"/>
-      <c r="I2" s="121" t="s">
+      <c r="I2" s="116" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="122" t="s">
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="117" t="s">
         <v>82</v>
       </c>
-      <c r="N2" s="122"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="122"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
       <c r="Q2" s="51"/>
-      <c r="R2" s="115" t="s">
+      <c r="R2" s="123" t="s">
         <v>83</v>
       </c>
-      <c r="S2" s="114" t="s">
+      <c r="S2" s="122" t="s">
         <v>84</v>
       </c>
-      <c r="T2" s="114"/>
-      <c r="U2" s="114"/>
+      <c r="T2" s="122"/>
+      <c r="U2" s="122"/>
       <c r="V2" s="50"/>
       <c r="W2" s="29"/>
       <c r="X2" s="29"/>
-      <c r="Y2" s="112" t="s">
+      <c r="Y2" s="120" t="s">
         <v>85</v>
       </c>
-      <c r="Z2" s="112"/>
-      <c r="AA2" s="112" t="s">
+      <c r="Z2" s="120"/>
+      <c r="AA2" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="AB2" s="112"/>
+      <c r="AB2" s="120"/>
     </row>
     <row r="3" spans="1:28" s="30" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="37"/>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="121" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="113"/>
-      <c r="F3" s="123" t="s">
+      <c r="E3" s="121"/>
+      <c r="F3" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="123"/>
+      <c r="G3" s="118"/>
       <c r="H3" s="26"/>
       <c r="I3" s="38"/>
-      <c r="J3" s="119" t="s">
+      <c r="J3" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
+      <c r="K3" s="115"/>
+      <c r="L3" s="115"/>
       <c r="M3" s="38"/>
-      <c r="N3" s="119" t="s">
+      <c r="N3" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="O3" s="120"/>
-      <c r="P3" s="120"/>
+      <c r="O3" s="115"/>
+      <c r="P3" s="115"/>
       <c r="Q3" s="47"/>
-      <c r="R3" s="115"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="114"/>
-      <c r="U3" s="114"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="122"/>
+      <c r="T3" s="122"/>
+      <c r="U3" s="122"/>
       <c r="V3" s="50"/>
       <c r="W3" s="31"/>
       <c r="X3" s="31"/>
-      <c r="Y3" s="112"/>
-      <c r="Z3" s="112"/>
-      <c r="AA3" s="112"/>
-      <c r="AB3" s="112"/>
+      <c r="Y3" s="120"/>
+      <c r="Z3" s="120"/>
+      <c r="AA3" s="120"/>
+      <c r="AB3" s="120"/>
     </row>
     <row r="4" spans="1:28" s="2" customFormat="1" ht="53.65" customHeight="1">
       <c r="A4" s="33" t="s">
@@ -11004,7 +11018,7 @@
       <c r="V5" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="W5" s="101" t="s">
+      <c r="W5" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X5" s="6" t="s">
@@ -11090,7 +11104,7 @@
       <c r="V6" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="W6" s="101" t="s">
+      <c r="W6" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X6" s="6" t="s">
@@ -11176,7 +11190,7 @@
       <c r="V7" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="W7" s="101" t="s">
+      <c r="W7" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X7" s="6" t="s">
@@ -11262,7 +11276,7 @@
       <c r="V8" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="W8" s="101" t="s">
+      <c r="W8" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X8" s="6" t="s">
@@ -11348,7 +11362,7 @@
       <c r="V9" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="W9" s="101" t="s">
+      <c r="W9" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X9" s="6" t="s">
@@ -11434,7 +11448,7 @@
       <c r="V10" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="W10" s="101" t="s">
+      <c r="W10" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X10" s="6" t="s">
@@ -11520,7 +11534,7 @@
       <c r="V11" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="W11" s="101" t="s">
+      <c r="W11" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X11" s="6" t="s">
@@ -11606,7 +11620,7 @@
       <c r="V12" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="W12" s="101" t="s">
+      <c r="W12" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X12" s="6" t="s">
@@ -11692,7 +11706,7 @@
       <c r="V13" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="W13" s="101" t="s">
+      <c r="W13" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X13" s="6" t="s">
@@ -12208,7 +12222,7 @@
       <c r="V19" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W19" s="101" t="s">
+      <c r="W19" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X19" s="6" t="s">
@@ -12294,7 +12308,7 @@
       <c r="V20" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W20" s="101" t="s">
+      <c r="W20" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X20" s="6" t="s">
@@ -12380,7 +12394,7 @@
       <c r="V21" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W21" s="101" t="s">
+      <c r="W21" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X21" s="6" t="s">
@@ -12466,7 +12480,7 @@
       <c r="V22" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W22" s="101" t="s">
+      <c r="W22" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X22" s="6" t="s">
@@ -12552,7 +12566,7 @@
       <c r="V23" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W23" s="101" t="s">
+      <c r="W23" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X23" s="6" t="s">
@@ -12638,7 +12652,7 @@
       <c r="V24" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W24" s="101" t="s">
+      <c r="W24" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X24" s="6" t="s">
@@ -12724,7 +12738,7 @@
       <c r="V25" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W25" s="101" t="s">
+      <c r="W25" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X25" s="6" t="s">
@@ -12810,7 +12824,7 @@
       <c r="V26" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W26" s="101" t="s">
+      <c r="W26" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X26" s="6" t="s">
@@ -12896,7 +12910,7 @@
       <c r="V27" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W27" s="101" t="s">
+      <c r="W27" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X27" s="6" t="s">
@@ -12982,7 +12996,7 @@
       <c r="V28" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="W28" s="101" t="s">
+      <c r="W28" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X28" s="6" t="s">
@@ -13068,7 +13082,7 @@
       <c r="V29" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="W29" s="101" t="s">
+      <c r="W29" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X29" s="6" t="s">
@@ -13154,7 +13168,7 @@
       <c r="V30" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W30" s="101" t="s">
+      <c r="W30" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X30" s="6" t="s">
@@ -13240,7 +13254,7 @@
       <c r="V31" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W31" s="101" t="s">
+      <c r="W31" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X31" s="6" t="s">
@@ -13326,7 +13340,7 @@
       <c r="V32" s="39" t="s">
         <v>438</v>
       </c>
-      <c r="W32" s="101" t="s">
+      <c r="W32" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X32" s="6" t="s">
@@ -13412,7 +13426,7 @@
       <c r="V33" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W33" s="101" t="s">
+      <c r="W33" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X33" s="6" t="s">
@@ -13498,7 +13512,7 @@
       <c r="V34" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="W34" s="101" t="s">
+      <c r="W34" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X34" s="6" t="s">
@@ -13584,7 +13598,7 @@
       <c r="V35" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W35" s="101" t="s">
+      <c r="W35" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X35" s="6" t="s">
@@ -13670,7 +13684,7 @@
       <c r="V36" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W36" s="101" t="s">
+      <c r="W36" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X36" s="6" t="s">
@@ -13756,7 +13770,7 @@
       <c r="V37" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W37" s="101" t="s">
+      <c r="W37" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X37" s="6" t="s">
@@ -13842,7 +13856,7 @@
       <c r="V38" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W38" s="101" t="s">
+      <c r="W38" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X38" s="6" t="s">
@@ -13928,7 +13942,7 @@
       <c r="V39" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W39" s="101" t="s">
+      <c r="W39" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X39" s="6" t="s">
@@ -14014,7 +14028,7 @@
       <c r="V40" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W40" s="101" t="s">
+      <c r="W40" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X40" s="42" t="s">
@@ -14100,7 +14114,7 @@
       <c r="V41" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W41" s="101" t="s">
+      <c r="W41" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X41" s="42" t="s">
@@ -14186,7 +14200,7 @@
       <c r="V42" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W42" s="101" t="s">
+      <c r="W42" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X42" s="42" t="s">
@@ -14272,7 +14286,7 @@
       <c r="V43" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W43" s="101" t="s">
+      <c r="W43" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X43" s="42" t="s">
@@ -14358,7 +14372,7 @@
       <c r="V44" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W44" s="101" t="s">
+      <c r="W44" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X44" s="42" t="s">
@@ -14444,7 +14458,7 @@
       <c r="V45" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W45" s="101" t="s">
+      <c r="W45" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X45" s="42" t="s">
@@ -14530,7 +14544,7 @@
       <c r="V46" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W46" s="101" t="s">
+      <c r="W46" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X46" s="42" t="s">
@@ -14616,7 +14630,7 @@
       <c r="V47" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W47" s="101" t="s">
+      <c r="W47" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X47" s="42" t="s">
@@ -14702,7 +14716,7 @@
       <c r="V48" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W48" s="101" t="s">
+      <c r="W48" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X48" s="42" t="s">
@@ -14788,7 +14802,7 @@
       <c r="V49" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W49" s="101" t="s">
+      <c r="W49" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X49" s="42" t="s">
@@ -14874,7 +14888,7 @@
       <c r="V50" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W50" s="101" t="s">
+      <c r="W50" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X50" s="42" t="s">
@@ -14960,7 +14974,7 @@
       <c r="V51" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W51" s="101" t="s">
+      <c r="W51" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X51" s="42" t="s">
@@ -15046,7 +15060,7 @@
       <c r="V52" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W52" s="101" t="s">
+      <c r="W52" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X52" s="42" t="s">
@@ -15132,7 +15146,7 @@
       <c r="V53" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W53" s="101" t="s">
+      <c r="W53" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X53" s="42" t="s">
@@ -15218,7 +15232,7 @@
       <c r="V54" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W54" s="101" t="s">
+      <c r="W54" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X54" s="6" t="s">
@@ -15304,7 +15318,7 @@
       <c r="V55" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W55" s="101" t="s">
+      <c r="W55" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X55" s="6" t="s">
@@ -15390,7 +15404,7 @@
       <c r="V56" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W56" s="101" t="s">
+      <c r="W56" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X56" s="42" t="s">
@@ -15476,7 +15490,7 @@
       <c r="V57" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W57" s="101" t="s">
+      <c r="W57" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X57" s="42" t="s">
@@ -15562,7 +15576,7 @@
       <c r="V58" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W58" s="101" t="s">
+      <c r="W58" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X58" s="42" t="s">
@@ -15648,7 +15662,7 @@
       <c r="V59" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W59" s="101" t="s">
+      <c r="W59" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X59" s="42" t="s">
@@ -15734,7 +15748,7 @@
       <c r="V60" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W60" s="101" t="s">
+      <c r="W60" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X60" s="42" t="s">
@@ -15820,7 +15834,7 @@
       <c r="V61" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W61" s="101" t="s">
+      <c r="W61" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X61" s="42" t="s">
@@ -15906,7 +15920,7 @@
       <c r="V62" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W62" s="101" t="s">
+      <c r="W62" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X62" s="42" t="s">
@@ -15992,7 +16006,7 @@
       <c r="V63" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W63" s="101" t="s">
+      <c r="W63" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X63" s="42" t="s">
@@ -16078,7 +16092,7 @@
       <c r="V64" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W64" s="101" t="s">
+      <c r="W64" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X64" s="42" t="s">
@@ -16164,7 +16178,7 @@
       <c r="V65" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W65" s="101" t="s">
+      <c r="W65" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X65" s="42" t="s">
@@ -16250,7 +16264,7 @@
       <c r="V66" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W66" s="101" t="s">
+      <c r="W66" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X66" s="42" t="s">
@@ -16336,7 +16350,7 @@
       <c r="V67" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W67" s="101" t="s">
+      <c r="W67" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X67" s="42" t="s">
@@ -16422,7 +16436,7 @@
       <c r="V68" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W68" s="101" t="s">
+      <c r="W68" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X68" s="42" t="s">
@@ -16508,7 +16522,7 @@
       <c r="V69" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W69" s="101" t="s">
+      <c r="W69" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X69" s="42" t="s">
@@ -16594,7 +16608,7 @@
       <c r="V70" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W70" s="101" t="s">
+      <c r="W70" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X70" s="42" t="s">
@@ -16680,7 +16694,7 @@
       <c r="V71" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W71" s="101" t="s">
+      <c r="W71" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X71" s="42" t="s">
@@ -16766,7 +16780,7 @@
       <c r="V72" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W72" s="101" t="s">
+      <c r="W72" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X72" s="42" t="s">
@@ -16852,7 +16866,7 @@
       <c r="V73" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W73" s="101" t="s">
+      <c r="W73" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X73" s="42" t="s">
@@ -16938,7 +16952,7 @@
       <c r="V74" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W74" s="101" t="s">
+      <c r="W74" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X74" s="42" t="s">
@@ -17024,7 +17038,7 @@
       <c r="V75" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="W75" s="101" t="s">
+      <c r="W75" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X75" s="42" t="s">
@@ -17110,7 +17124,7 @@
       <c r="V76" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W76" s="101" t="s">
+      <c r="W76" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X76" s="42" t="s">
@@ -17196,7 +17210,7 @@
       <c r="V77" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W77" s="101" t="s">
+      <c r="W77" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X77" s="42" t="s">
@@ -17282,7 +17296,7 @@
       <c r="V78" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W78" s="101" t="s">
+      <c r="W78" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X78" s="42" t="s">
@@ -17368,7 +17382,7 @@
       <c r="V79" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W79" s="101" t="s">
+      <c r="W79" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X79" s="42" t="s">
@@ -17454,7 +17468,7 @@
       <c r="V80" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W80" s="101" t="s">
+      <c r="W80" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X80" s="42" t="s">
@@ -17540,7 +17554,7 @@
       <c r="V81" s="39" t="s">
         <v>958</v>
       </c>
-      <c r="W81" s="101" t="s">
+      <c r="W81" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X81" s="42" t="s">
@@ -17626,7 +17640,7 @@
       <c r="V82" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W82" s="101" t="s">
+      <c r="W82" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X82" s="42" t="s">
@@ -17712,7 +17726,7 @@
       <c r="V83" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W83" s="101" t="s">
+      <c r="W83" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X83" s="42" t="s">
@@ -18228,7 +18242,7 @@
       <c r="V89" s="39" t="s">
         <v>958</v>
       </c>
-      <c r="W89" s="101" t="s">
+      <c r="W89" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X89" s="42" t="s">
@@ -18314,7 +18328,7 @@
       <c r="V90" s="39" t="s">
         <v>958</v>
       </c>
-      <c r="W90" s="101" t="s">
+      <c r="W90" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X90" s="42" t="s">
@@ -18400,7 +18414,7 @@
       <c r="V91" s="39" t="s">
         <v>958</v>
       </c>
-      <c r="W91" s="101" t="s">
+      <c r="W91" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X91" s="42" t="s">
@@ -18486,7 +18500,7 @@
       <c r="V92" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W92" s="101" t="s">
+      <c r="W92" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X92" s="42" t="s">
@@ -18572,7 +18586,7 @@
       <c r="V93" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W93" s="101" t="s">
+      <c r="W93" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X93" s="42" t="s">
@@ -18658,7 +18672,7 @@
       <c r="V94" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W94" s="101" t="s">
+      <c r="W94" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X94" s="42" t="s">
@@ -18744,7 +18758,7 @@
       <c r="V95" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W95" s="101" t="s">
+      <c r="W95" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X95" s="42" t="s">
@@ -18830,7 +18844,7 @@
       <c r="V96" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W96" s="101" t="s">
+      <c r="W96" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X96" s="42" t="s">
@@ -18916,7 +18930,7 @@
       <c r="V97" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W97" s="101" t="s">
+      <c r="W97" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X97" s="42" t="s">
@@ -19002,7 +19016,7 @@
       <c r="V98" s="39" t="s">
         <v>438</v>
       </c>
-      <c r="W98" s="101" t="s">
+      <c r="W98" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X98" s="42" t="s">
@@ -19088,7 +19102,7 @@
       <c r="V99" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W99" s="101" t="s">
+      <c r="W99" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X99" s="42" t="s">
@@ -19174,7 +19188,7 @@
       <c r="V100" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W100" s="101" t="s">
+      <c r="W100" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X100" s="42" t="s">
@@ -19260,7 +19274,7 @@
       <c r="V101" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W101" s="101" t="s">
+      <c r="W101" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X101" s="42" t="s">
@@ -19346,7 +19360,7 @@
       <c r="V102" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="W102" s="101" t="s">
+      <c r="W102" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X102" s="42" t="s">
@@ -19432,7 +19446,7 @@
       <c r="V103" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W103" s="101" t="s">
+      <c r="W103" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X103" s="42" t="s">
@@ -19518,7 +19532,7 @@
       <c r="V104" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="W104" s="101" t="s">
+      <c r="W104" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X104" s="42" t="s">
@@ -19604,7 +19618,7 @@
       <c r="V105" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W105" s="101" t="s">
+      <c r="W105" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X105" s="42" t="s">
@@ -19690,7 +19704,7 @@
       <c r="V106" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W106" s="101" t="s">
+      <c r="W106" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X106" s="42" t="s">
@@ -19776,7 +19790,7 @@
       <c r="V107" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W107" s="101" t="s">
+      <c r="W107" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X107" s="42" t="s">
@@ -19862,10 +19876,10 @@
       <c r="V108" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W108" s="101" t="s">
+      <c r="W108" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="X108" s="101" t="s">
+      <c r="X108" s="100" t="s">
         <v>1155</v>
       </c>
       <c r="Y108" s="22" t="s">
@@ -19948,10 +19962,10 @@
       <c r="V109" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="W109" s="101" t="s">
+      <c r="W109" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="X109" s="101" t="s">
+      <c r="X109" s="100" t="s">
         <v>528</v>
       </c>
       <c r="Y109" s="22" t="s">
@@ -20034,7 +20048,7 @@
       <c r="V110" s="39" t="s">
         <v>1174</v>
       </c>
-      <c r="W110" s="101" t="s">
+      <c r="W110" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X110" s="42" t="s">
@@ -20120,7 +20134,7 @@
       <c r="V111" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="W111" s="101" t="s">
+      <c r="W111" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X111" s="42" t="s">
@@ -20206,7 +20220,7 @@
       <c r="V112" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="W112" s="101" t="s">
+      <c r="W112" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X112" s="42" t="s">
@@ -20292,7 +20306,7 @@
       <c r="V113" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="W113" s="101" t="s">
+      <c r="W113" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X113" s="42" t="s">
@@ -20378,7 +20392,7 @@
       <c r="V114" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="W114" s="101" t="s">
+      <c r="W114" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X114" s="42" t="s">
@@ -20446,7 +20460,7 @@
       <c r="P115" s="2" t="s">
         <v>1220</v>
       </c>
-      <c r="Q115" s="124" t="s">
+      <c r="Q115" s="101" t="s">
         <v>1221</v>
       </c>
       <c r="R115" s="42" t="s">
@@ -20464,7 +20478,7 @@
       <c r="V115" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W115" s="101" t="s">
+      <c r="W115" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X115" s="42" t="s">
@@ -20532,7 +20546,7 @@
       <c r="P116" s="2" t="s">
         <v>1233</v>
       </c>
-      <c r="Q116" s="124" t="s">
+      <c r="Q116" s="101" t="s">
         <v>1234</v>
       </c>
       <c r="R116" s="42" t="s">
@@ -20550,7 +20564,7 @@
       <c r="V116" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W116" s="101" t="s">
+      <c r="W116" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X116" s="42" t="s">
@@ -20618,7 +20632,7 @@
       <c r="P117" s="2" t="s">
         <v>2747</v>
       </c>
-      <c r="Q117" s="124" t="s">
+      <c r="Q117" s="101" t="s">
         <v>1243</v>
       </c>
       <c r="R117" s="42" t="s">
@@ -20636,7 +20650,7 @@
       <c r="V117" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W117" s="101" t="s">
+      <c r="W117" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X117" s="42" t="s">
@@ -20704,7 +20718,7 @@
       <c r="P118" s="42" t="s">
         <v>976</v>
       </c>
-      <c r="Q118" s="124" t="s">
+      <c r="Q118" s="101" t="s">
         <v>1253</v>
       </c>
       <c r="R118" s="42" t="s">
@@ -20722,7 +20736,7 @@
       <c r="V118" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W118" s="101" t="s">
+      <c r="W118" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X118" s="42" t="s">
@@ -20808,7 +20822,7 @@
       <c r="V119" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="W119" s="101" t="s">
+      <c r="W119" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X119" s="42" t="s">
@@ -20894,7 +20908,7 @@
       <c r="V120" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="W120" s="101" t="s">
+      <c r="W120" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X120" s="42" t="s">
@@ -20980,7 +20994,7 @@
       <c r="V121" s="39" t="s">
         <v>1279</v>
       </c>
-      <c r="W121" s="101" t="s">
+      <c r="W121" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X121" s="42" t="s">
@@ -21066,7 +21080,7 @@
       <c r="V122" s="39" t="s">
         <v>1279</v>
       </c>
-      <c r="W122" s="101" t="s">
+      <c r="W122" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X122" s="42" t="s">
@@ -21152,7 +21166,7 @@
       <c r="V123" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="W123" s="101" t="s">
+      <c r="W123" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X123" s="42" t="s">
@@ -21238,7 +21252,7 @@
       <c r="V124" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W124" s="101" t="s">
+      <c r="W124" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X124" s="42" t="s">
@@ -21324,7 +21338,7 @@
       <c r="V125" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W125" s="101" t="s">
+      <c r="W125" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X125" s="42" t="s">
@@ -21410,7 +21424,7 @@
       <c r="V126" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W126" s="101" t="s">
+      <c r="W126" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X126" s="42" t="s">
@@ -21496,7 +21510,7 @@
       <c r="V127" s="39" t="s">
         <v>1174</v>
       </c>
-      <c r="W127" s="101" t="s">
+      <c r="W127" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X127" s="42" t="s">
@@ -21582,7 +21596,7 @@
       <c r="V128" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W128" s="101" t="s">
+      <c r="W128" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X128" s="42" t="s">
@@ -21668,7 +21682,7 @@
       <c r="V129" s="39" t="s">
         <v>1350</v>
       </c>
-      <c r="W129" s="101" t="s">
+      <c r="W129" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X129" s="42" t="s">
@@ -21754,7 +21768,7 @@
       <c r="V130" s="39" t="s">
         <v>1174</v>
       </c>
-      <c r="W130" s="101" t="s">
+      <c r="W130" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X130" s="42" t="s">
@@ -21840,7 +21854,7 @@
       <c r="V131" s="39" t="s">
         <v>1174</v>
       </c>
-      <c r="W131" s="101" t="s">
+      <c r="W131" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X131" s="42" t="s">
@@ -21926,7 +21940,7 @@
       <c r="V132" s="39" t="s">
         <v>2805</v>
       </c>
-      <c r="W132" s="101" t="s">
+      <c r="W132" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X132" s="42" t="s">
@@ -21994,7 +22008,7 @@
       <c r="P133" s="2" t="s">
         <v>1220</v>
       </c>
-      <c r="Q133" s="124" t="s">
+      <c r="Q133" s="101" t="s">
         <v>1386</v>
       </c>
       <c r="R133" s="42" t="s">
@@ -22012,7 +22026,7 @@
       <c r="V133" s="39" t="s">
         <v>1279</v>
       </c>
-      <c r="W133" s="101" t="s">
+      <c r="W133" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X133" s="42" t="s">
@@ -22080,7 +22094,7 @@
       <c r="P134" s="2" t="s">
         <v>1398</v>
       </c>
-      <c r="Q134" s="124" t="s">
+      <c r="Q134" s="101" t="s">
         <v>1399</v>
       </c>
       <c r="R134" s="42" t="s">
@@ -22098,7 +22112,7 @@
       <c r="V134" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="W134" s="101" t="s">
+      <c r="W134" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X134" s="42" t="s">
@@ -22166,7 +22180,7 @@
       <c r="P135" s="2" t="s">
         <v>1409</v>
       </c>
-      <c r="Q135" s="124" t="s">
+      <c r="Q135" s="101" t="s">
         <v>1410</v>
       </c>
       <c r="R135" s="42" t="s">
@@ -22184,7 +22198,7 @@
       <c r="V135" s="39" t="s">
         <v>1174</v>
       </c>
-      <c r="W135" s="101" t="s">
+      <c r="W135" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X135" s="42" t="s">
@@ -22252,7 +22266,7 @@
       <c r="P136" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q136" s="124" t="s">
+      <c r="Q136" s="101" t="s">
         <v>1420</v>
       </c>
       <c r="R136" s="42" t="s">
@@ -22270,7 +22284,7 @@
       <c r="V136" s="39" t="s">
         <v>1424</v>
       </c>
-      <c r="W136" s="101" t="s">
+      <c r="W136" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X136" s="42" t="s">
@@ -22338,7 +22352,7 @@
       <c r="P137" s="2" t="s">
         <v>1220</v>
       </c>
-      <c r="Q137" s="124" t="s">
+      <c r="Q137" s="101" t="s">
         <v>1430</v>
       </c>
       <c r="R137" s="42" t="s">
@@ -22356,7 +22370,7 @@
       <c r="V137" s="39" t="s">
         <v>1424</v>
       </c>
-      <c r="W137" s="101" t="s">
+      <c r="W137" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X137" s="42" t="s">
@@ -22424,7 +22438,7 @@
       <c r="P138" s="2" t="s">
         <v>2747</v>
       </c>
-      <c r="Q138" s="124" t="s">
+      <c r="Q138" s="101" t="s">
         <v>1437</v>
       </c>
       <c r="R138" s="42" t="s">
@@ -22442,7 +22456,7 @@
       <c r="V138" s="39" t="s">
         <v>1442</v>
       </c>
-      <c r="W138" s="101" t="s">
+      <c r="W138" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X138" s="42" t="s">
@@ -22510,7 +22524,7 @@
       <c r="P139" s="42" t="s">
         <v>2747</v>
       </c>
-      <c r="Q139" s="124" t="s">
+      <c r="Q139" s="101" t="s">
         <v>1447</v>
       </c>
       <c r="R139" s="42" t="s">
@@ -22528,7 +22542,7 @@
       <c r="V139" s="39" t="s">
         <v>1424</v>
       </c>
-      <c r="W139" s="101" t="s">
+      <c r="W139" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X139" s="42" t="s">
@@ -22596,7 +22610,7 @@
       <c r="P140" s="2" t="s">
         <v>1344</v>
       </c>
-      <c r="Q140" s="124" t="s">
+      <c r="Q140" s="101" t="s">
         <v>1456</v>
       </c>
       <c r="R140" s="42" t="s">
@@ -22614,7 +22628,7 @@
       <c r="V140" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="W140" s="101" t="s">
+      <c r="W140" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X140" s="42" t="s">
@@ -22682,7 +22696,7 @@
       <c r="P141" s="42" t="s">
         <v>1465</v>
       </c>
-      <c r="Q141" s="124" t="s">
+      <c r="Q141" s="101" t="s">
         <v>1466</v>
       </c>
       <c r="R141" s="42" t="s">
@@ -22700,7 +22714,7 @@
       <c r="V141" s="39" t="s">
         <v>1174</v>
       </c>
-      <c r="W141" s="101" t="s">
+      <c r="W141" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X141" s="42" t="s">
@@ -22768,7 +22782,7 @@
       <c r="P142" s="2" t="s">
         <v>1398</v>
       </c>
-      <c r="Q142" s="124" t="s">
+      <c r="Q142" s="101" t="s">
         <v>1474</v>
       </c>
       <c r="R142" s="42" t="s">
@@ -22786,7 +22800,7 @@
       <c r="V142" s="39" t="s">
         <v>1225</v>
       </c>
-      <c r="W142" s="101" t="s">
+      <c r="W142" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X142" s="42" t="s">
@@ -22854,7 +22868,7 @@
       <c r="P143" s="2" t="s">
         <v>1483</v>
       </c>
-      <c r="Q143" s="124" t="s">
+      <c r="Q143" s="101" t="s">
         <v>1484</v>
       </c>
       <c r="R143" s="42" t="s">
@@ -22872,7 +22886,7 @@
       <c r="V143" s="39" t="s">
         <v>1174</v>
       </c>
-      <c r="W143" s="101" t="s">
+      <c r="W143" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X143" s="42" t="s">
@@ -22940,7 +22954,7 @@
       <c r="P144" s="2" t="s">
         <v>1483</v>
       </c>
-      <c r="Q144" s="124" t="s">
+      <c r="Q144" s="101" t="s">
         <v>1492</v>
       </c>
       <c r="R144" s="42" t="s">
@@ -22958,7 +22972,7 @@
       <c r="V144" s="39" t="s">
         <v>1174</v>
       </c>
-      <c r="W144" s="101" t="s">
+      <c r="W144" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X144" s="42" t="s">
@@ -23044,7 +23058,7 @@
       <c r="V145" s="2" t="s">
         <v>1506</v>
       </c>
-      <c r="W145" s="101" t="s">
+      <c r="W145" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X145" s="42" t="s">
@@ -23130,7 +23144,7 @@
       <c r="V146" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="W146" s="101" t="s">
+      <c r="W146" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X146" s="42" t="s">
@@ -23216,7 +23230,7 @@
       <c r="V147" s="2" t="s">
         <v>1528</v>
       </c>
-      <c r="W147" s="101" t="s">
+      <c r="W147" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X147" s="42" t="s">
@@ -23302,7 +23316,7 @@
       <c r="V148" s="2" t="s">
         <v>1538</v>
       </c>
-      <c r="W148" s="101" t="s">
+      <c r="W148" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X148" s="42" t="s">
@@ -23388,7 +23402,7 @@
       <c r="V149" s="2" t="s">
         <v>1549</v>
       </c>
-      <c r="W149" s="101" t="s">
+      <c r="W149" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X149" s="42" t="s">
@@ -23474,7 +23488,7 @@
       <c r="V150" s="2" t="s">
         <v>1561</v>
       </c>
-      <c r="W150" s="101" t="s">
+      <c r="W150" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X150" s="42" t="s">
@@ -23560,7 +23574,7 @@
       <c r="V151" s="2" t="s">
         <v>958</v>
       </c>
-      <c r="W151" s="101" t="s">
+      <c r="W151" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X151" s="42" t="s">
@@ -23646,7 +23660,7 @@
       <c r="V152" s="2" t="s">
         <v>958</v>
       </c>
-      <c r="W152" s="101" t="s">
+      <c r="W152" s="100" t="s">
         <v>209</v>
       </c>
       <c r="X152" s="42" t="s">
@@ -23732,7 +23746,7 @@
       <c r="V153" s="2" t="s">
         <v>1561</v>
       </c>
-      <c r="W153" s="101" t="s">
+      <c r="W153" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X153" s="42" t="s">
@@ -23818,7 +23832,7 @@
       <c r="V154" s="2" t="s">
         <v>1598</v>
       </c>
-      <c r="W154" s="101" t="s">
+      <c r="W154" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X154" s="42" t="s">
@@ -23904,7 +23918,7 @@
       <c r="V155" s="2" t="s">
         <v>1528</v>
       </c>
-      <c r="W155" s="101" t="s">
+      <c r="W155" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X155" s="42" t="s">
@@ -23990,7 +24004,7 @@
       <c r="V156" s="2" t="s">
         <v>1538</v>
       </c>
-      <c r="W156" s="101" t="s">
+      <c r="W156" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X156" s="42" t="s">
@@ -24076,7 +24090,7 @@
       <c r="V157" s="2" t="s">
         <v>1538</v>
       </c>
-      <c r="W157" s="101" t="s">
+      <c r="W157" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X157" s="42" t="s">
@@ -24162,7 +24176,7 @@
       <c r="V158" s="2" t="s">
         <v>1528</v>
       </c>
-      <c r="W158" s="101" t="s">
+      <c r="W158" s="100" t="s">
         <v>251</v>
       </c>
       <c r="X158" s="42" t="s">
@@ -24248,7 +24262,7 @@
       <c r="V159" s="2" t="s">
         <v>958</v>
       </c>
-      <c r="W159" s="101" t="s">
+      <c r="W159" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X159" s="42" t="s">
@@ -24334,7 +24348,7 @@
       <c r="V160" s="2" t="s">
         <v>1561</v>
       </c>
-      <c r="W160" s="101" t="s">
+      <c r="W160" s="100" t="s">
         <v>122</v>
       </c>
       <c r="X160" s="42" t="s">
@@ -52755,6 +52769,12 @@
     <sortCondition ref="C5:C284"/>
   </sortState>
   <mergeCells count="16">
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="Y2:Z3"/>
+    <mergeCell ref="AA2:AB3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="S2:U3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="D1:H1"/>
@@ -52765,12 +52785,6 @@
     <mergeCell ref="I1:R1"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="Y2:Z3"/>
-    <mergeCell ref="AA2:AB3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="S2:U3"/>
-    <mergeCell ref="R2:R3"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:D18">
     <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
@@ -53124,15 +53138,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c70d178-d21c-48a3-aa0e-ddb58e3b7295">
@@ -53143,6 +53148,15 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53166,14 +53180,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC43FB1-6F13-4FC9-A3DC-D5E732E9F9F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32E97209-EA28-4125-8A8D-2BD814449A59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -53183,4 +53189,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CC43FB1-6F13-4FC9-A3DC-D5E732E9F9F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>